<commit_message>
Sensitivity analysis on energy mix.
</commit_message>
<xml_diff>
--- a/files/LCI_CW.xlsx
+++ b/files/LCI_CW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0F1639-EAB1-4643-9CF7-98A28EB22230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB110D6E-11B7-42DA-8A14-CB23CF9A068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" activeTab="1" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" firstSheet="45" activeTab="48" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5193" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5207" uniqueCount="428">
   <si>
     <t>skip</t>
   </si>
@@ -1236,9 +1236,6 @@
     <t>market for used curtain wall, aluminium frame, low performance, for double glazing</t>
   </si>
   <si>
-    <t>exldb_cw_EoL</t>
-  </si>
-  <si>
     <t>BE_market_eol_cw_lowperf_dg</t>
   </si>
   <si>
@@ -1333,6 +1330,42 @@
   </si>
   <si>
     <t>param_ext_shdg_device + param_int_shdg_device</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_lowperf_sg</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_lowperf_dg</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_highperf_dg</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_highperf_tg</t>
+  </si>
+  <si>
+    <t>be_market_eol_ccf</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_vacuum</t>
+  </si>
+  <si>
+    <t>be_market_eol_cw_smart</t>
+  </si>
+  <si>
+    <t>be_market_eol_dsf</t>
+  </si>
+  <si>
+    <t>exldb_cw_eol</t>
+  </si>
+  <si>
+    <t>market for used screen, metalised blind fabric</t>
+  </si>
+  <si>
+    <t>-(param_int_shdg_device + param_ext_shdg_device)</t>
+  </si>
+  <si>
+    <t>be_market_eol_screen</t>
   </si>
 </sst>
 </file>
@@ -4008,11 +4041,13 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
@@ -6257,8 +6292,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6423,7 +6458,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -6438,7 +6473,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -6447,7 +6482,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O15"/>
     </row>
@@ -14959,7 +14994,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15691,7 +15726,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16568,7 +16603,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16724,7 +16759,7 @@
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="23" t="s">
-        <v>384</v>
+        <v>424</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -16754,7 +16789,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -16768,7 +16803,7 @@
         <v>72</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>71</v>
@@ -17661,7 +17696,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17693,7 +17728,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -17709,7 +17744,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -17807,7 +17842,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B12" s="40">
         <v>1</v>
@@ -17847,7 +17882,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -17862,7 +17897,7 @@
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="23" t="s">
-        <v>384</v>
+        <v>424</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -17892,7 +17927,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -18060,7 +18095,7 @@
         <v>72</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>71</v>
@@ -19489,15 +19524,15 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F3D49-74C2-4BFC-A6B6-5745C01BC058}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
@@ -19524,7 +19559,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19540,7 +19575,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -19638,7 +19673,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -19647,10 +19682,10 @@
         <v>72</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -19680,12 +19715,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>191</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -19694,10 +19729,10 @@
         <v>72</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -19727,7 +19762,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>198</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -19741,10 +19776,10 @@
         <v>72</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>64</v>
@@ -19774,12 +19809,12 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>203</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -19788,10 +19823,10 @@
         <v>72</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>64</v>
@@ -19821,12 +19856,12 @@
         <v>64</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>208</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B16" s="40">
         <v>0</v>
@@ -19835,10 +19870,10 @@
         <v>72</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>64</v>
@@ -19868,12 +19903,12 @@
         <v>64</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>288</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B17" s="40">
         <v>0</v>
@@ -19882,10 +19917,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>64</v>
@@ -19915,12 +19950,12 @@
         <v>64</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>214</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -19929,10 +19964,10 @@
         <v>72</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>64</v>
@@ -19962,12 +19997,12 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>222</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -19976,10 +20011,10 @@
         <v>72</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>64</v>
@@ -20009,12 +20044,12 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>225</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -20023,10 +20058,10 @@
         <v>72</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>64</v>
@@ -20056,12 +20091,12 @@
         <v>64</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>294</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -20070,10 +20105,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>64</v>
@@ -20103,12 +20138,12 @@
         <v>64</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>304</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -20117,10 +20152,10 @@
         <v>72</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>64</v>
@@ -20150,12 +20185,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>317</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -20164,10 +20199,10 @@
         <v>72</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>64</v>
@@ -20197,12 +20232,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>327</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -20211,10 +20246,10 @@
         <v>72</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>64</v>
@@ -20244,12 +20279,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>232</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -20258,10 +20293,10 @@
         <v>72</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>64</v>
@@ -20291,22 +20326,24 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="B26" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="49" t="s">
+        <v>426</v>
+      </c>
       <c r="E26" s="23" t="s">
-        <v>71</v>
+        <v>424</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>64</v>
@@ -20315,30 +20352,75 @@
         <v>45</v>
       </c>
       <c r="H26" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O26" s="23" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" s="40">
+        <v>1</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="I26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>407</v>
-      </c>
-      <c r="P26" s="24"/>
+      <c r="I27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O27" s="23" t="s">
+        <v>406</v>
+      </c>
+      <c r="P27" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>